<commit_message>
The SPARC4 spectral response was implemented
</commit_message>
<xml_diff>
--- a/AIS/SPARC4_Spectral_Response/Channel 0/camera.xlsx
+++ b/AIS/SPARC4_Spectral_Response/Channel 0/camera.xlsx
@@ -20,9 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">camera</t>
+    <t xml:space="preserve">Wavelength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmitance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(nm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(%)</t>
   </si>
 </sst>
 </file>
@@ -110,16 +119,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,82 +157,187 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.78125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.83"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="A3" s="3" t="n">
+        <v>350</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
+      <c r="A4" s="3" t="n">
+        <f aca="false">A3+50</f>
+        <v>400</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="n">
+      <c r="A5" s="3" t="n">
+        <f aca="false">A4+50</f>
+        <v>450</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <f aca="false">A5+50</f>
+        <v>500</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <f aca="false">A6+50</f>
+        <v>550</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <f aca="false">A7+50</f>
+        <v>600</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <f aca="false">A8+50</f>
+        <v>650</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <f aca="false">A9+50</f>
+        <v>700</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <f aca="false">A10+50</f>
+        <v>750</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="n">
+        <f aca="false">A11+50</f>
+        <v>800</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
+        <f aca="false">A12+50</f>
+        <v>850</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <f aca="false">A13+50</f>
+        <v>900</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
+        <f aca="false">A14+50</f>
+        <v>950</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
+        <f aca="false">A15+50</f>
+        <v>1000</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
+        <f aca="false">A16+50</f>
+        <v>1050</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
+        <f aca="false">A17+50</f>
+        <v>1100</v>
+      </c>
+      <c r="B18" s="3" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added the extra ordinary ray for polarimetric acquisitions
</commit_message>
<xml_diff>
--- a/AIS/SPARC4_Spectral_Response/Channel 0/camera.xlsx
+++ b/AIS/SPARC4_Spectral_Response/Channel 0/camera.xlsx
@@ -160,7 +160,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -193,7 +193,7 @@
         <v>350</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -204,7 +204,7 @@
         <v>400</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -215,7 +215,7 @@
         <v>450</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -226,7 +226,7 @@
         <v>500</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,7 +235,7 @@
         <v>550</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,7 +244,7 @@
         <v>600</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,7 +253,7 @@
         <v>650</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,7 +262,7 @@
         <v>700</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -271,7 +271,7 @@
         <v>750</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,7 +280,7 @@
         <v>800</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,7 +289,7 @@
         <v>850</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +298,7 @@
         <v>900</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,7 +307,7 @@
         <v>950</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,7 +316,7 @@
         <v>1000</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,7 +325,7 @@
         <v>1050</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,7 +334,7 @@
         <v>1100</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>